<commit_message>
Actualizacion final con metrica F1
</commit_message>
<xml_diff>
--- a/salidas/importances.xlsx
+++ b/salidas/importances.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -455,7 +455,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.1860857490751982</v>
+        <v>0.1547037571708041</v>
       </c>
     </row>
     <row r="3">
@@ -464,11 +464,11 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>EnvironmentSatisfaction</t>
+          <t>DistanceFromHome</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.08266308963874175</v>
+        <v>0.1256262200658769</v>
       </c>
     </row>
     <row r="4">
@@ -477,11 +477,11 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>MonthlyIncome</t>
+          <t>EnvironmentSatisfaction</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.3787781137462094</v>
+        <v>0.07180021619067051</v>
       </c>
     </row>
     <row r="5">
@@ -490,11 +490,11 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>NumCompaniesWorked</t>
+          <t>MonthlyIncome</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.09287385596467798</v>
+        <v>0.231762606920802</v>
       </c>
     </row>
     <row r="6">
@@ -503,11 +503,11 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>TotalWorkingYears</t>
+          <t>NumCompaniesWorked</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.1589039265435407</v>
+        <v>0.08045655969826347</v>
       </c>
     </row>
     <row r="7">
@@ -516,11 +516,37 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
+          <t>PercentSalaryHike</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>0.1078954508922652</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>TotalWorkingYears</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>0.1317218604522631</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
           <t>YearsAtCompany</t>
         </is>
       </c>
-      <c r="C7" t="n">
-        <v>0.1006952650316318</v>
+      <c r="C9" t="n">
+        <v>0.09603332860905472</v>
       </c>
     </row>
   </sheetData>

</xml_diff>